<commit_message>
checking changes from my window machine
</commit_message>
<xml_diff>
--- a/my1stProject/processor/processor.xlsx
+++ b/my1stProject/processor/processor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoC\demo\processor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anupam\git\hello-world\my1stProject\processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="767">
   <si>
     <t>Component Name</t>
   </si>
@@ -2614,6 +2614,9 @@
   </si>
   <si>
     <t>AddressSpaces</t>
+  </si>
+  <si>
+    <t>addinf information</t>
   </si>
 </sst>
 </file>
@@ -4090,10 +4093,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5224,7 +5227,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="216"/>
+      <c r="B3" s="217"/>
       <c r="C3" s="111"/>
       <c r="D3" s="112"/>
       <c r="E3" s="113"/>
@@ -5238,8 +5241,8 @@
       <c r="M3" s="117"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="216"/>
-      <c r="C4" s="216"/>
+      <c r="B4" s="217"/>
+      <c r="C4" s="217"/>
       <c r="D4" s="218"/>
       <c r="E4" s="219"/>
       <c r="F4" s="114"/>
@@ -5252,8 +5255,8 @@
       <c r="M4" s="117"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="216"/>
-      <c r="C5" s="216"/>
+      <c r="B5" s="217"/>
+      <c r="C5" s="217"/>
       <c r="D5" s="218"/>
       <c r="E5" s="219"/>
       <c r="F5" s="114"/>
@@ -5266,8 +5269,8 @@
       <c r="M5" s="117"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="216"/>
-      <c r="C6" s="216"/>
+      <c r="B6" s="217"/>
+      <c r="C6" s="217"/>
       <c r="D6" s="218"/>
       <c r="E6" s="219"/>
       <c r="F6" s="114"/>
@@ -5280,8 +5283,8 @@
       <c r="M6" s="117"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="216"/>
-      <c r="C7" s="216"/>
+      <c r="B7" s="217"/>
+      <c r="C7" s="217"/>
       <c r="D7" s="218"/>
       <c r="E7" s="219"/>
       <c r="F7" s="114"/>
@@ -5294,8 +5297,8 @@
       <c r="M7" s="117"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="216"/>
-      <c r="C8" s="216"/>
+      <c r="B8" s="217"/>
+      <c r="C8" s="217"/>
       <c r="D8" s="218"/>
       <c r="E8" s="219"/>
       <c r="F8" s="114"/>
@@ -5308,7 +5311,7 @@
       <c r="M8" s="123"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="216"/>
+      <c r="B9" s="217"/>
       <c r="C9" s="91"/>
       <c r="D9" s="112"/>
       <c r="E9" s="113"/>
@@ -5322,7 +5325,7 @@
       <c r="M9" s="123"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="216"/>
+      <c r="B10" s="217"/>
       <c r="C10" s="111"/>
       <c r="D10" s="112"/>
       <c r="E10" s="113"/>
@@ -5336,7 +5339,7 @@
       <c r="M10" s="112"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="216"/>
+      <c r="B11" s="217"/>
       <c r="C11" s="125"/>
       <c r="D11" s="117"/>
       <c r="E11" s="126"/>
@@ -5350,8 +5353,8 @@
       <c r="M11" s="117"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="217"/>
-      <c r="C12" s="216"/>
+      <c r="B12" s="216"/>
+      <c r="C12" s="217"/>
       <c r="D12" s="218"/>
       <c r="E12" s="113"/>
       <c r="F12" s="114"/>
@@ -5364,8 +5367,8 @@
       <c r="M12" s="123"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="217"/>
-      <c r="C13" s="216"/>
+      <c r="B13" s="216"/>
+      <c r="C13" s="217"/>
       <c r="D13" s="218"/>
       <c r="E13" s="113"/>
       <c r="F13" s="114"/>
@@ -5378,8 +5381,8 @@
       <c r="M13" s="123"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="217"/>
-      <c r="C14" s="216"/>
+      <c r="B14" s="216"/>
+      <c r="C14" s="217"/>
       <c r="D14" s="218"/>
       <c r="E14" s="113"/>
       <c r="F14" s="114"/>
@@ -5392,8 +5395,8 @@
       <c r="M14" s="123"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="217"/>
-      <c r="C15" s="216"/>
+      <c r="B15" s="216"/>
+      <c r="C15" s="217"/>
       <c r="D15" s="218"/>
       <c r="E15" s="113"/>
       <c r="F15" s="114"/>
@@ -5406,8 +5409,8 @@
       <c r="M15" s="123"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="217"/>
-      <c r="C16" s="216"/>
+      <c r="B16" s="216"/>
+      <c r="C16" s="217"/>
       <c r="D16" s="218"/>
       <c r="E16" s="113"/>
       <c r="F16" s="114"/>
@@ -5420,8 +5423,8 @@
       <c r="M16" s="123"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="217"/>
-      <c r="C17" s="216"/>
+      <c r="B17" s="216"/>
+      <c r="C17" s="217"/>
       <c r="D17" s="218"/>
       <c r="E17" s="113"/>
       <c r="F17" s="114"/>
@@ -5434,8 +5437,8 @@
       <c r="M17" s="123"/>
     </row>
     <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="217"/>
-      <c r="C18" s="216"/>
+      <c r="B18" s="216"/>
+      <c r="C18" s="217"/>
       <c r="D18" s="218"/>
       <c r="E18" s="113"/>
       <c r="F18" s="114"/>
@@ -5448,8 +5451,8 @@
       <c r="M18" s="123"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="217"/>
-      <c r="C19" s="216"/>
+      <c r="B19" s="216"/>
+      <c r="C19" s="217"/>
       <c r="D19" s="218"/>
       <c r="E19" s="113"/>
       <c r="F19" s="114"/>
@@ -5505,12 +5508,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B15"/>
@@ -5521,6 +5518,12 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7922,7 +7925,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7994,7 +7997,9 @@
       <c r="D3" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="86" t="s">
+        <v>766</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>

</xml_diff>